<commit_message>
add the split the data
</commit_message>
<xml_diff>
--- a/raw_data/airport_choice_survey_EN_ver2.0_Capstone.xlsx
+++ b/raw_data/airport_choice_survey_EN_ver2.0_Capstone.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leem\Documents\Capstone\airport choice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuai\Repository\data_mining_group\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D51D31-F412-47BB-9A18-D83E1E5D005E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="168" windowWidth="20352" windowHeight="7872"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="303">
   <si>
     <t>ID</t>
   </si>
@@ -568,12 +569,6 @@
     <t>JL974</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>W7667</t>
-  </si>
-  <si>
     <t>KE2727</t>
   </si>
   <si>
@@ -944,7 +939,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
@@ -1164,32 +1159,14 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1200,12 +1177,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="표준 2" xfId="1"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,6 +1291,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1331,6 +1343,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1506,101 +1535,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB489"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B388" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="O400" sqref="O400"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28" s="34" customFormat="1" ht="43.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:28" s="26" customFormat="1" ht="45">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="34" t="s">
+      <c r="J1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="X1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AA1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AB1" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -32051,10 +32080,7 @@
         <v>3</v>
       </c>
       <c r="O400" t="s">
-        <v>181</v>
-      </c>
-      <c r="P400" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="Q400">
         <v>11</v>
@@ -32297,7 +32323,7 @@
         <v>2</v>
       </c>
       <c r="O403" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P403">
         <v>16</v>
@@ -32522,7 +32548,7 @@
         <v>1</v>
       </c>
       <c r="O406" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P406">
         <v>8</v>
@@ -32904,7 +32930,7 @@
         <v>1</v>
       </c>
       <c r="O411" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P411">
         <v>12</v>
@@ -33852,7 +33878,7 @@
         <v>1</v>
       </c>
       <c r="O423" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P423">
         <v>8</v>
@@ -34012,7 +34038,7 @@
         <v>2</v>
       </c>
       <c r="O425" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P425">
         <v>15</v>
@@ -34089,7 +34115,7 @@
         <v>2</v>
       </c>
       <c r="O426" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P426">
         <v>16</v>
@@ -34166,7 +34192,7 @@
         <v>2</v>
       </c>
       <c r="O427" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P427">
         <v>16</v>
@@ -35031,7 +35057,7 @@
         <v>3</v>
       </c>
       <c r="O438" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="P438">
         <v>13</v>
@@ -35268,7 +35294,7 @@
         <v>1</v>
       </c>
       <c r="O441" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P441">
         <v>12</v>
@@ -35671,7 +35697,7 @@
         <v>1</v>
       </c>
       <c r="O446" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P446">
         <v>12</v>
@@ -36059,7 +36085,7 @@
         <v>2</v>
       </c>
       <c r="O451" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P451">
         <v>12</v>
@@ -36222,7 +36248,7 @@
         <v>2</v>
       </c>
       <c r="O453" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P453">
         <v>16</v>
@@ -36385,7 +36411,7 @@
         <v>1</v>
       </c>
       <c r="O455" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P455">
         <v>19</v>
@@ -36459,7 +36485,7 @@
         <v>1</v>
       </c>
       <c r="O456" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P456">
         <v>19</v>
@@ -36536,7 +36562,7 @@
         <v>2</v>
       </c>
       <c r="O457" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P457">
         <v>16</v>
@@ -37214,7 +37240,7 @@
         <v>2</v>
       </c>
       <c r="O466" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P466">
         <v>16</v>
@@ -37933,7 +37959,7 @@
         <v>2</v>
       </c>
       <c r="O476" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P476">
         <v>20</v>
@@ -38010,7 +38036,7 @@
         <v>2</v>
       </c>
       <c r="O477" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P477">
         <v>20</v>
@@ -38386,7 +38412,7 @@
         <v>1</v>
       </c>
       <c r="O482" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P482">
         <v>19</v>
@@ -38614,7 +38640,7 @@
         <v>1</v>
       </c>
       <c r="O485" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P485">
         <v>19</v>
@@ -38848,7 +38874,7 @@
         <v>2</v>
       </c>
       <c r="O488" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P488">
         <v>19</v>
@@ -38971,33 +38997,34 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB489" xr:uid="{961C6ED5-EEE0-4BF4-95A1-1D15C5AD7F9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C175"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="30" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="20" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="4" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="A1" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="22"/>
@@ -39005,28 +39032,28 @@
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="A3" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="19" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="A7" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4"/>
@@ -39035,28 +39062,28 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="9"/>
@@ -39067,17 +39094,17 @@
       <c r="C13" s="7"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B15" s="26"/>
+      <c r="A15" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="32"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5"/>
@@ -39086,14 +39113,14 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -39104,11 +39131,11 @@
       <c r="C22" s="7"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
+      <c r="A25" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4"/>
@@ -39117,155 +39144,155 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="9"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" ht="22.8">
+    <row r="36" spans="1:3" ht="24">
       <c r="A36" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="9"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="B42" s="33"/>
+      <c r="A42" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" s="34"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="B45" s="30"/>
+      <c r="A45" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
+      <c r="A49" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B51" s="14"/>
       <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="9"/>
@@ -39281,31 +39308,31 @@
       <c r="C59" s="7"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
+      <c r="A62" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="9"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="B67" s="31"/>
+      <c r="A67" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B67" s="35"/>
       <c r="C67" s="17"/>
     </row>
     <row r="68" spans="1:3">
@@ -39315,11 +39342,11 @@
       <c r="C69" s="18"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
+      <c r="A70" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="4"/>
@@ -39328,84 +39355,84 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B78" s="16"/>
       <c r="C78" s="9"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="B82" s="29"/>
-      <c r="C82" s="30"/>
+      <c r="A82" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B82" s="36"/>
+      <c r="C82" s="28"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="9"/>
@@ -39421,25 +39448,25 @@
       <c r="C90" s="25"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B91" s="32"/>
+      <c r="C91" s="32"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="6"/>
@@ -39447,64 +39474,64 @@
       <c r="C96" s="6"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-    </row>
-    <row r="98" spans="1:3" ht="14.4">
+      <c r="A97" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+    </row>
+    <row r="98" spans="1:3" ht="15">
       <c r="A98" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" ht="14.4">
+    <row r="99" spans="1:3" ht="15">
       <c r="A99" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" ht="14.4">
+    <row r="100" spans="1:3" ht="15">
       <c r="A100" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" ht="14.4">
+    <row r="101" spans="1:3" ht="15">
       <c r="A101" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="22"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="28" t="s">
-        <v>295</v>
-      </c>
-      <c r="B104" s="29"/>
-      <c r="C104" s="30"/>
+      <c r="A104" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="B104" s="36"/>
+      <c r="C104" s="28"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="9"/>
@@ -39515,23 +39542,23 @@
       <c r="C108" s="7"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B110" s="28"/>
+    </row>
+    <row r="113" spans="1:3" ht="32.65" customHeight="1">
+      <c r="A113" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="B113" s="32"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="B110" s="30"/>
-    </row>
-    <row r="113" spans="1:3" ht="32.700000000000003" customHeight="1">
-      <c r="A113" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="B113" s="26"/>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
+      <c r="B116" s="32"/>
+      <c r="C116" s="32"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="4"/>
@@ -39540,100 +39567,100 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B118" s="12"/>
       <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B119" s="12"/>
       <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B121" s="12"/>
       <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B122" s="12"/>
       <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B123" s="12"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B124" s="12"/>
       <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B125" s="12"/>
       <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B126" s="12"/>
       <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B127" s="12"/>
       <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B128" s="12"/>
       <c r="C128" s="9"/>
     </row>
-    <row r="131" spans="1:3" ht="31.8" customHeight="1">
-      <c r="A131" s="35" t="s">
+    <row r="131" spans="1:3" ht="31.9" customHeight="1">
+      <c r="A131" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" s="30"/>
+      <c r="C131" s="31"/>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B134" s="32"/>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="B131" s="36"/>
-      <c r="C131" s="37"/>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B134" s="26"/>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="B137" s="26"/>
-      <c r="C137" s="26"/>
+      <c r="B137" s="32"/>
+      <c r="C137" s="32"/>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="5"/>
@@ -39642,84 +39669,84 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="9"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B140" s="14"/>
       <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B141" s="14"/>
       <c r="C141" s="9"/>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B143" s="14"/>
       <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B144" s="14"/>
       <c r="C144" s="9"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="9"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="9"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B147" s="14"/>
       <c r="C147" s="9"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B148" s="14"/>
       <c r="C148" s="9"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B149" s="14"/>
       <c r="C149" s="9"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B150" s="14"/>
       <c r="C150" s="9"/>
@@ -39730,11 +39757,11 @@
       <c r="C151" s="7"/>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="B154" s="26"/>
-      <c r="C154" s="26"/>
+      <c r="A154" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="B154" s="32"/>
+      <c r="C154" s="32"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="5"/>
@@ -39743,59 +39770,59 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="9"/>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B157" s="14"/>
       <c r="C157" s="9"/>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B158" s="14"/>
       <c r="C158" s="9"/>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="9"/>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="9"/>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B161" s="14"/>
       <c r="C161" s="9"/>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="9"/>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="26" t="s">
-        <v>303</v>
-      </c>
-      <c r="B165" s="26"/>
-      <c r="C165" s="26"/>
+      <c r="A165" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="B165" s="32"/>
+      <c r="C165" s="32"/>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="4"/>
@@ -39804,35 +39831,35 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B167" s="14"/>
       <c r="C167" s="9"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="9"/>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B169" s="14"/>
       <c r="C169" s="9"/>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B170" s="14"/>
       <c r="C170" s="9"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B171" s="14"/>
       <c r="C171" s="9"/>
@@ -39844,29 +39871,16 @@
       <c r="B173" s="21"/>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="27" t="s">
-        <v>304</v>
-      </c>
-      <c r="B174" s="27"/>
+      <c r="A174" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="B174" s="37"/>
     </row>
     <row r="175" spans="1:3">
       <c r="B175" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A82:C82"/>
     <mergeCell ref="A154:C154"/>
     <mergeCell ref="A165:C165"/>
     <mergeCell ref="A174:B174"/>
@@ -39882,6 +39896,19 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A82:C82"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updata some data wrangling code
</commit_message>
<xml_diff>
--- a/raw_data/airport_choice_survey_EN_ver2.0_Capstone.xlsx
+++ b/raw_data/airport_choice_survey_EN_ver2.0_Capstone.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuai\Repository\data_mining_group\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leem\Documents\Capstone\airport choice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D51D31-F412-47BB-9A18-D83E1E5D005E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="168" windowWidth="20352" windowHeight="7872"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="305">
   <si>
     <t>ID</t>
   </si>
@@ -569,6 +568,12 @@
     <t>JL974</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W7667</t>
+  </si>
+  <si>
     <t>KE2727</t>
   </si>
   <si>
@@ -939,7 +944,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
@@ -1159,14 +1164,32 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1177,30 +1200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="표준 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="표준 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1291,23 +1296,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1343,23 +1331,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1535,101 +1506,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB489"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B388" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O400" sqref="O400"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:28" s="26" customFormat="1" ht="45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:28" s="34" customFormat="1" ht="43.2">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="26" t="s">
+      <c r="D1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>268</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="26" t="s">
+      <c r="F1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="V1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="W1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Y1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AA1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AB1" s="34" t="s">
         <v>22</v>
       </c>
     </row>
@@ -32080,7 +32051,10 @@
         <v>3</v>
       </c>
       <c r="O400" t="s">
-        <v>141</v>
+        <v>181</v>
+      </c>
+      <c r="P400" t="s">
+        <v>182</v>
       </c>
       <c r="Q400">
         <v>11</v>
@@ -32323,7 +32297,7 @@
         <v>2</v>
       </c>
       <c r="O403" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P403">
         <v>16</v>
@@ -32548,7 +32522,7 @@
         <v>1</v>
       </c>
       <c r="O406" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="P406">
         <v>8</v>
@@ -32930,7 +32904,7 @@
         <v>1</v>
       </c>
       <c r="O411" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="P411">
         <v>12</v>
@@ -33878,7 +33852,7 @@
         <v>1</v>
       </c>
       <c r="O423" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P423">
         <v>8</v>
@@ -34038,7 +34012,7 @@
         <v>2</v>
       </c>
       <c r="O425" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="P425">
         <v>15</v>
@@ -34115,7 +34089,7 @@
         <v>2</v>
       </c>
       <c r="O426" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="P426">
         <v>16</v>
@@ -34192,7 +34166,7 @@
         <v>2</v>
       </c>
       <c r="O427" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="P427">
         <v>16</v>
@@ -35057,7 +35031,7 @@
         <v>3</v>
       </c>
       <c r="O438" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="P438">
         <v>13</v>
@@ -35294,7 +35268,7 @@
         <v>1</v>
       </c>
       <c r="O441" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P441">
         <v>12</v>
@@ -35697,7 +35671,7 @@
         <v>1</v>
       </c>
       <c r="O446" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P446">
         <v>12</v>
@@ -36085,7 +36059,7 @@
         <v>2</v>
       </c>
       <c r="O451" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="P451">
         <v>12</v>
@@ -36248,7 +36222,7 @@
         <v>2</v>
       </c>
       <c r="O453" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P453">
         <v>16</v>
@@ -36411,7 +36385,7 @@
         <v>1</v>
       </c>
       <c r="O455" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P455">
         <v>19</v>
@@ -36485,7 +36459,7 @@
         <v>1</v>
       </c>
       <c r="O456" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P456">
         <v>19</v>
@@ -36562,7 +36536,7 @@
         <v>2</v>
       </c>
       <c r="O457" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P457">
         <v>16</v>
@@ -37240,7 +37214,7 @@
         <v>2</v>
       </c>
       <c r="O466" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="P466">
         <v>16</v>
@@ -37959,7 +37933,7 @@
         <v>2</v>
       </c>
       <c r="O476" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="P476">
         <v>20</v>
@@ -38036,7 +38010,7 @@
         <v>2</v>
       </c>
       <c r="O477" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="P477">
         <v>20</v>
@@ -38412,7 +38386,7 @@
         <v>1</v>
       </c>
       <c r="O482" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="P482">
         <v>19</v>
@@ -38640,7 +38614,7 @@
         <v>1</v>
       </c>
       <c r="O485" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="P485">
         <v>19</v>
@@ -38874,7 +38848,7 @@
         <v>2</v>
       </c>
       <c r="O488" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="P488">
         <v>19</v>
@@ -38997,34 +38971,33 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB489" xr:uid="{961C6ED5-EEE0-4BF4-95A1-1D15C5AD7F9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C175"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A147" workbookViewId="0">
       <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <cols>
     <col min="1" max="1" width="30" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="20" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="3"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="A1" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="22"/>
@@ -39032,28 +39005,28 @@
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="A3" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="19" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="19" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="32" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
+      <c r="A7" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4"/>
@@ -39062,28 +39035,28 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="9"/>
@@ -39094,17 +39067,17 @@
       <c r="C13" s="7"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" s="32"/>
+      <c r="A15" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="26"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5"/>
@@ -39113,14 +39086,14 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -39131,11 +39104,11 @@
       <c r="C22" s="7"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="A25" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4"/>
@@ -39144,155 +39117,155 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="11" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="9"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
+      <c r="A34" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" ht="24">
+    <row r="36" spans="1:3" ht="22.8">
       <c r="A36" s="11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="11" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="9"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="B42" s="34"/>
+      <c r="A42" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B42" s="33"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B45" s="28"/>
+      <c r="A45" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B45" s="30"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="19" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
+      <c r="A49" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B51" s="14"/>
       <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="11" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="11" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="15" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="15" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="9"/>
@@ -39308,31 +39281,31 @@
       <c r="C59" s="7"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
+      <c r="A62" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="9"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="35" t="s">
-        <v>279</v>
-      </c>
-      <c r="B67" s="35"/>
+      <c r="A67" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="B67" s="31"/>
       <c r="C67" s="17"/>
     </row>
     <row r="68" spans="1:3">
@@ -39342,11 +39315,11 @@
       <c r="C69" s="18"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
+      <c r="A70" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="4"/>
@@ -39355,84 +39328,84 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B78" s="16"/>
       <c r="C78" s="9"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B82" s="36"/>
-      <c r="C82" s="28"/>
+      <c r="A82" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="B82" s="29"/>
+      <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="9"/>
@@ -39448,25 +39421,25 @@
       <c r="C90" s="25"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
+      <c r="A91" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
+      <c r="A93" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32"/>
+      <c r="A95" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="6"/>
@@ -39474,64 +39447,64 @@
       <c r="C96" s="6"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="32" t="s">
-        <v>292</v>
-      </c>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-    </row>
-    <row r="98" spans="1:3" ht="15">
+      <c r="A97" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+    </row>
+    <row r="98" spans="1:3" ht="14.4">
       <c r="A98" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" ht="15">
+    <row r="99" spans="1:3" ht="14.4">
       <c r="A99" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" ht="15">
+    <row r="100" spans="1:3" ht="14.4">
       <c r="A100" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" ht="15">
+    <row r="101" spans="1:3" ht="14.4">
       <c r="A101" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="22"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="B104" s="36"/>
-      <c r="C104" s="28"/>
+      <c r="A104" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B104" s="29"/>
+      <c r="C104" s="30"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="9"/>
@@ -39542,23 +39515,23 @@
       <c r="C108" s="7"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="B110" s="28"/>
-    </row>
-    <row r="113" spans="1:3" ht="32.65" customHeight="1">
-      <c r="A113" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="B113" s="32"/>
+      <c r="A110" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B110" s="30"/>
+    </row>
+    <row r="113" spans="1:3" ht="32.700000000000003" customHeight="1">
+      <c r="A113" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="B113" s="26"/>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32"/>
+      <c r="A116" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B116" s="26"/>
+      <c r="C116" s="26"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="4"/>
@@ -39567,100 +39540,100 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B118" s="12"/>
       <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B119" s="12"/>
       <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B121" s="12"/>
       <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B122" s="12"/>
       <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B123" s="12"/>
       <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B124" s="12"/>
       <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B125" s="12"/>
       <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B126" s="12"/>
       <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B127" s="12"/>
       <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B128" s="12"/>
       <c r="C128" s="9"/>
     </row>
-    <row r="131" spans="1:3" ht="31.9" customHeight="1">
-      <c r="A131" s="29" t="s">
-        <v>297</v>
-      </c>
-      <c r="B131" s="30"/>
-      <c r="C131" s="31"/>
+    <row r="131" spans="1:3" ht="31.8" customHeight="1">
+      <c r="A131" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="B131" s="36"/>
+      <c r="C131" s="37"/>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="32" t="s">
-        <v>298</v>
-      </c>
-      <c r="B134" s="32"/>
+      <c r="A134" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B134" s="26"/>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="B137" s="32"/>
-      <c r="C137" s="32"/>
+      <c r="A137" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="B137" s="26"/>
+      <c r="C137" s="26"/>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="5"/>
@@ -39669,84 +39642,84 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="9"/>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B140" s="14"/>
       <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B141" s="14"/>
       <c r="C141" s="9"/>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B143" s="14"/>
       <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B144" s="14"/>
       <c r="C144" s="9"/>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="9"/>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B146" s="14"/>
       <c r="C146" s="9"/>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B147" s="14"/>
       <c r="C147" s="9"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B148" s="14"/>
       <c r="C148" s="9"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B149" s="14"/>
       <c r="C149" s="9"/>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B150" s="14"/>
       <c r="C150" s="9"/>
@@ -39757,11 +39730,11 @@
       <c r="C151" s="7"/>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="32" t="s">
-        <v>300</v>
-      </c>
-      <c r="B154" s="32"/>
-      <c r="C154" s="32"/>
+      <c r="A154" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="B154" s="26"/>
+      <c r="C154" s="26"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="5"/>
@@ -39770,59 +39743,59 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="9"/>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B157" s="14"/>
       <c r="C157" s="9"/>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B158" s="14"/>
       <c r="C158" s="9"/>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="9"/>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B160" s="14"/>
       <c r="C160" s="9"/>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B161" s="14"/>
       <c r="C161" s="9"/>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B162" s="14"/>
       <c r="C162" s="9"/>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="B165" s="32"/>
-      <c r="C165" s="32"/>
+      <c r="A165" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="B165" s="26"/>
+      <c r="C165" s="26"/>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="4"/>
@@ -39831,35 +39804,35 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B167" s="14"/>
       <c r="C167" s="9"/>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="9"/>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B169" s="14"/>
       <c r="C169" s="9"/>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B170" s="14"/>
       <c r="C170" s="9"/>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B171" s="14"/>
       <c r="C171" s="9"/>
@@ -39871,16 +39844,29 @@
       <c r="B173" s="21"/>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="B174" s="37"/>
+      <c r="A174" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="B174" s="27"/>
     </row>
     <row r="175" spans="1:3">
       <c r="B175" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A82:C82"/>
     <mergeCell ref="A154:C154"/>
     <mergeCell ref="A165:C165"/>
     <mergeCell ref="A174:B174"/>
@@ -39896,19 +39882,6 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A82:C82"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>